<commit_message>
atts de produto e excel
</commit_message>
<xml_diff>
--- a/Desenvolvimento Ajol.xlsx
+++ b/Desenvolvimento Ajol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProjetoAjol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD47C877-B5A3-414D-A596-AD41079578B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385BF711-57D1-4B41-92B1-161A7E9BE274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{776A3329-5419-4B5C-81A0-7DF2732FC879}"/>
   </bookViews>
@@ -35,6 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>GABRIEL DEIRO DOS SANTOS</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{985147B9-7AD8-4F89-A17C-BD25ADEDF153}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Testar anexo de imagens no cadastro</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
@@ -126,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +165,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -527,11 +558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A061C2C-E535-42E9-A0B8-7369B43EBF63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A061C2C-E535-42E9-A0B8-7369B43EBF63}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,5 +679,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>